<commit_message>
Corrected JDBC-statements for adding vendors
</commit_message>
<xml_diff>
--- a/SnelStartVendorExport0001.xlsx
+++ b/SnelStartVendorExport0001.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>guid</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>terms0003</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>taxtable0003</t>
@@ -162,8 +165,8 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -217,11 +220,11 @@
       <c r="P1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="0" t="n">
-        <v>1</v>
+      <c r="Q1" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Importing of Customers and Vendors working
</commit_message>
<xml_diff>
--- a/SnelStartVendorExport0001.xlsx
+++ b/SnelStartVendorExport0001.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>guid</t>
   </si>
@@ -56,10 +56,7 @@
     <t>email0001</t>
   </si>
   <si>
-    <t>terms0001</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>YES</t>
   </si>
   <si>
     <t>taxtable0001</t>
@@ -101,7 +98,7 @@
     <t>email0002</t>
   </si>
   <si>
-    <t>terms0002</t>
+    <t>NO</t>
   </si>
   <si>
     <t>taxtable0002</t>
@@ -207,8 +204,8 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -262,14 +259,14 @@
       <c r="O1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -277,55 +274,55 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimization in retrieving generated uuids
</commit_message>
<xml_diff>
--- a/SnelStartVendorExport0001.xlsx
+++ b/SnelStartVendorExport0001.xlsx
@@ -59,7 +59,7 @@
     <t>YES</t>
   </si>
   <si>
-    <t>taxtable0001</t>
+    <t>Hoog</t>
   </si>
   <si>
     <t>Naam0002</t>
@@ -101,7 +101,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>taxtable0002</t>
+    <t>Laag</t>
   </si>
 </sst>
 </file>
@@ -204,8 +204,8 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Names Vendors more expliciet
</commit_message>
<xml_diff>
--- a/SnelStartVendorExport0001.xlsx
+++ b/SnelStartVendorExport0001.xlsx
@@ -20,7 +20,7 @@
     <t>guid</t>
   </si>
   <si>
-    <t>Naam0001</t>
+    <t>LeverancierNaam0001</t>
   </si>
   <si>
     <t>id0001</t>
@@ -62,7 +62,7 @@
     <t>Hoog</t>
   </si>
   <si>
-    <t>Naam0002</t>
+    <t>LeverancierNaam0002</t>
   </si>
   <si>
     <t>id0002</t>
@@ -204,8 +204,8 @@
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>